<commit_message>
Adding inferred data to excel sheet and mapping correlations
</commit_message>
<xml_diff>
--- a/Quarantine Survey(1-90).xlsx
+++ b/Quarantine Survey(1-90).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alan\Documents\Quarantine-Lifestyle-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B027890-FCAC-4783-B694-72CD43036C76}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2283301-400B-4D2C-9F56-349528496CBD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId3"/>
+    <pivotCache cacheId="0" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="54">
   <si>
     <t>ID</t>
   </si>
@@ -183,6 +183,21 @@
   <si>
     <t>What was the completion time?</t>
   </si>
+  <si>
+    <t>Do you work or attend class for at least 15 hours per week?</t>
+  </si>
+  <si>
+    <t>Do you live with other people?</t>
+  </si>
+  <si>
+    <t>Do you live with more than 1 person?</t>
+  </si>
+  <si>
+    <t>Do you work or attend class more than 40 hours a week?</t>
+  </si>
+  <si>
+    <t>Do you have pets?</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +277,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
+  <dxfs count="35">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -270,10 +285,31 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FFFFC000"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -289,21 +325,6 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FFFFC000"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -538,6 +559,15 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -6008,7 +6038,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CAF45BE-4D5E-4372-9529-6ACCD65D5CA7}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9CAF45BE-4D5E-4372-9529-6ACCD65D5CA7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="E12:F24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="28">
     <pivotField showAll="0"/>
@@ -6154,43 +6184,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AC91" totalsRowShown="0" headerRowDxfId="29">
-  <autoFilter ref="A1:AC91" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="29">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="How many hours a week do you currently work and/or attend class?" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="How many people do you currently live with?" dataDxfId="25"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="How many hours a week do you currently spend on making or fixing things as a hobby?" dataDxfId="24"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Do you have pets? How many?" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Do you feel like you decide how your day goes?" dataDxfId="22"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="How many hours a week do you currently spend studying outside of class?" dataDxfId="21"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="How many hours a week do you currently spend socializing with your social inner circle?" dataDxfId="20"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Do you currently work from home?" dataDxfId="19"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="How many hours a week do you currently spend exercising?" dataDxfId="18"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="At the end of the week, do you feel like you have more or less things on your To-do list?" dataDxfId="17"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Do you feel that the quarantine has made you more or less connected to others?" dataDxfId="16"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="How old are you?" dataDxfId="15"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="How many hours a week do you currently spend socializing with people who aren't in your inner circle, outside of work/class?" dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="How do you feel going throughout your day?" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="How many hours a night do you sleep?" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Do you feel that the quarantine has resulted in spending more or less time talking with your boss, teachers, and work peers?" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Do you feel like you decide what’s on your To-do list?" dataDxfId="10"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="How many hours a day do you spend outside?" dataDxfId="9"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Do you currently feel like you are more rested, or overworked?" dataDxfId="8"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="How many hours a week do you spend reading something you enjoy?" dataDxfId="7"/>
-    <tableColumn id="26" xr3:uid="{9946B6E0-47B0-4C03-A843-FCEDFF1B69F8}" name="." dataDxfId="6"/>
-    <tableColumn id="27" xr3:uid="{F08E3FE3-4F18-4DE6-BDD2-D16CB4A44517}" name="How many hours a week are accounted for?" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AH91" totalsRowShown="0" headerRowDxfId="34">
+  <autoFilter ref="A1:AH91" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="34">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="ID" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Start time" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Completion time" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Email" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Name" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="How many hours a week do you currently work and/or attend class?" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="How many people do you currently live with?" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="How many hours a week do you currently spend on making or fixing things as a hobby?" dataDxfId="26"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Do you have pets? How many?" dataDxfId="25"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Do you feel like you decide how your day goes?" dataDxfId="24"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="How many hours a week do you currently spend studying outside of class?" dataDxfId="23"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="How many hours a week do you currently spend socializing with your social inner circle?" dataDxfId="22"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Do you currently work from home?" dataDxfId="21"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="How many hours a week do you currently spend exercising?" dataDxfId="20"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="At the end of the week, do you feel like you have more or less things on your To-do list?" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Do you feel that the quarantine has made you more or less connected to others?" dataDxfId="18"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="How old are you?" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="How many hours a week do you currently spend socializing with people who aren't in your inner circle, outside of work/class?" dataDxfId="16"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="How do you feel going throughout your day?" dataDxfId="15"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="How many hours a night do you sleep?" dataDxfId="14"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="Do you feel that the quarantine has resulted in spending more or less time talking with your boss, teachers, and work peers?" dataDxfId="13"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="Do you feel like you decide what’s on your To-do list?" dataDxfId="12"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="How many hours a day do you spend outside?" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="Do you currently feel like you are more rested, or overworked?" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="How many hours a week do you spend reading something you enjoy?" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{9946B6E0-47B0-4C03-A843-FCEDFF1B69F8}" name="." dataDxfId="8"/>
+    <tableColumn id="27" xr3:uid="{F08E3FE3-4F18-4DE6-BDD2-D16CB4A44517}" name="How many hours a week are accounted for?" dataDxfId="7">
       <calculatedColumnFormula>SUM(F2,H2,K2, L2,N2,R2,(T2*7),(W2*7),Y2)/7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{956D6BF9-8597-4604-A601-3129427C4047}" name="What is the average Outlook score?" dataDxfId="5">
+    <tableColumn id="28" xr3:uid="{956D6BF9-8597-4604-A601-3129427C4047}" name="What is the average Outlook score?" dataDxfId="6">
       <calculatedColumnFormula>AVERAGE(J2,P2,S2,V2,X2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{79A1F31C-F938-4AD0-B34F-79123381EAB7}" name="What was the completion time?" dataDxfId="0">
+    <tableColumn id="29" xr3:uid="{79A1F31C-F938-4AD0-B34F-79123381EAB7}" name="What was the completion time?" dataDxfId="5">
       <calculatedColumnFormula>TEXT(C2-B2, "h:mm:ss")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="30" xr3:uid="{9A2C7940-588D-4407-A21C-268BD3C615DA}" name="Do you work or attend class for at least 15 hours per week?" dataDxfId="4">
+      <calculatedColumnFormula>IF(F2&gt;=15, 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="31" xr3:uid="{C08580A0-23A5-4DF6-B9C0-848DAA30F6F3}" name="Do you live with other people?" dataDxfId="3">
+      <calculatedColumnFormula>IF(G2&gt;0, 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="32" xr3:uid="{3F8A21B5-9C8A-43F4-853D-8E2BDE4F647E}" name="Do you live with more than 1 person?" dataDxfId="2">
+      <calculatedColumnFormula>IF(G2&gt;1, 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="33" xr3:uid="{27F26200-E124-4F90-B2EC-7532397146B7}" name="Do you work or attend class more than 40 hours a week?" dataDxfId="1">
+      <calculatedColumnFormula>IF(F2&gt;40, 1, 0)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="34" xr3:uid="{EC2003BB-4C4B-46B6-BDBF-A66A1134072F}" name="Do you have pets?" dataDxfId="0">
+      <calculatedColumnFormula>IF(I2&gt;0, 1, 0)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -6494,12 +6539,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC91"/>
+  <dimension ref="A1:AH91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="AD17" sqref="AD17"/>
+      <selection pane="bottomLeft" activeCell="AI12" sqref="AI12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6531,9 +6576,13 @@
     <col min="27" max="27" width="19.7109375" style="5" customWidth="1"/>
     <col min="28" max="28" width="19.7109375" style="6" customWidth="1"/>
     <col min="29" max="29" width="24" customWidth="1"/>
+    <col min="30" max="30" width="19.140625" customWidth="1"/>
+    <col min="31" max="31" width="18.28515625" customWidth="1"/>
+    <col min="32" max="32" width="16.85546875" customWidth="1"/>
+    <col min="33" max="33" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -6621,8 +6670,23 @@
       <c r="AC1" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="AD1" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="AE1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="AF1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH1" s="12" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6709,8 +6773,28 @@
         <f t="shared" ref="AC2:AC33" si="2">TEXT(C2-B2, "h:mm:ss")</f>
         <v>0:02:52</v>
       </c>
+      <c r="AD2">
+        <f t="shared" ref="AD2:AD33" si="3">IF(F2&gt;=15, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE2" s="3">
+        <f t="shared" ref="AE2:AE33" si="4">IF(G2&gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF2" s="3">
+        <f t="shared" ref="AF2:AF33" si="5">IF(G2&gt;1, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG2" s="3">
+        <f t="shared" ref="AG2:AG33" si="6">IF(F2&gt;40, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH2" s="3">
+        <f t="shared" ref="AH2:AH33" si="7">IF(I2&gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6797,8 +6881,28 @@
         <f t="shared" si="2"/>
         <v>0:02:49</v>
       </c>
+      <c r="AD3">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE3" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF3" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG3" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -6885,8 +6989,28 @@
         <f t="shared" si="2"/>
         <v>0:04:12</v>
       </c>
+      <c r="AD4">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE4" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF4" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG4" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH4" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -6973,8 +7097,28 @@
         <f t="shared" si="2"/>
         <v>0:02:50</v>
       </c>
+      <c r="AD5">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE5" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF5" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG5" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH5" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7061,8 +7205,28 @@
         <f t="shared" si="2"/>
         <v>0:12:08</v>
       </c>
+      <c r="AD6">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE6" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF6" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG6" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH6" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7149,8 +7313,28 @@
         <f t="shared" si="2"/>
         <v>0:04:45</v>
       </c>
+      <c r="AD7">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE7" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF7" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG7" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH7" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7237,8 +7421,28 @@
         <f t="shared" si="2"/>
         <v>0:33:16</v>
       </c>
+      <c r="AD8">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE8" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF8" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG8" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH8" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7325,8 +7529,28 @@
         <f t="shared" si="2"/>
         <v>0:02:24</v>
       </c>
+      <c r="AD9">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE9" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF9" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG9" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH9" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7413,8 +7637,28 @@
         <f t="shared" si="2"/>
         <v>0:02:33</v>
       </c>
+      <c r="AD10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE10" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF10" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG10" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH10" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7501,8 +7745,28 @@
         <f t="shared" si="2"/>
         <v>0:02:16</v>
       </c>
+      <c r="AD11">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE11" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF11" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG11" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH11" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7589,8 +7853,28 @@
         <f t="shared" si="2"/>
         <v>0:03:44</v>
       </c>
+      <c r="AD12">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE12" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF12" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG12" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH12" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7677,8 +7961,28 @@
         <f t="shared" si="2"/>
         <v>0:02:37</v>
       </c>
+      <c r="AD13">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE13" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF13" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG13" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH13" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7765,8 +8069,28 @@
         <f t="shared" si="2"/>
         <v>0:01:55</v>
       </c>
+      <c r="AD14">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE14" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF14" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG14" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH14" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7853,8 +8177,28 @@
         <f t="shared" si="2"/>
         <v>0:05:02</v>
       </c>
+      <c r="AD15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE15" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF15" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG15" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH15" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7941,8 +8285,28 @@
         <f t="shared" si="2"/>
         <v>0:04:00</v>
       </c>
+      <c r="AD16">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE16" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF16" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG16" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH16" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -8029,8 +8393,28 @@
         <f t="shared" si="2"/>
         <v>0:02:35</v>
       </c>
+      <c r="AD17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE17" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF17" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG17" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH17" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -8117,8 +8501,28 @@
         <f t="shared" si="2"/>
         <v>0:07:05</v>
       </c>
+      <c r="AD18">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE18" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF18" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG18" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH18" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -8205,8 +8609,28 @@
         <f t="shared" si="2"/>
         <v>0:02:46</v>
       </c>
+      <c r="AD19">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE19" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF19" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG19" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH19" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -8293,8 +8717,28 @@
         <f t="shared" si="2"/>
         <v>0:03:49</v>
       </c>
+      <c r="AD20">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE20" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF20" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG20" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH20" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -8381,8 +8825,28 @@
         <f t="shared" si="2"/>
         <v>0:10:54</v>
       </c>
+      <c r="AD21">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE21" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF21" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG21" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH21" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -8469,8 +8933,28 @@
         <f t="shared" si="2"/>
         <v>0:04:54</v>
       </c>
+      <c r="AD22">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE22" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF22" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG22" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH22" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -8557,8 +9041,28 @@
         <f t="shared" si="2"/>
         <v>0:09:18</v>
       </c>
+      <c r="AD23">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE23" s="3">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="AF23" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG23" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH23" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -8645,8 +9149,28 @@
         <f t="shared" si="2"/>
         <v>0:02:20</v>
       </c>
+      <c r="AD24">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE24" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF24" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG24" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH24" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -8733,8 +9257,28 @@
         <f t="shared" si="2"/>
         <v>0:09:37</v>
       </c>
+      <c r="AD25">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE25" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF25" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG25" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH25" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -8821,8 +9365,28 @@
         <f t="shared" si="2"/>
         <v>0:04:05</v>
       </c>
+      <c r="AD26">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE26" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF26" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG26" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH26" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -8909,8 +9473,28 @@
         <f t="shared" si="2"/>
         <v>0:02:20</v>
       </c>
+      <c r="AD27">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE27" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF27" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG27" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH27" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -8997,8 +9581,28 @@
         <f t="shared" si="2"/>
         <v>0:01:52</v>
       </c>
+      <c r="AD28">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE28" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF28" s="3">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AG28" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH28" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -9085,8 +9689,28 @@
         <f t="shared" si="2"/>
         <v>1:24:02</v>
       </c>
+      <c r="AD29">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE29" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF29" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG29" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH29" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -9173,8 +9797,28 @@
         <f t="shared" si="2"/>
         <v>0:04:50</v>
       </c>
+      <c r="AD30">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE30" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF30" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG30" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH30" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -9261,8 +9905,28 @@
         <f t="shared" si="2"/>
         <v>0:02:13</v>
       </c>
+      <c r="AD31">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE31" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF31" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG31" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH31" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -9349,8 +10013,28 @@
         <f t="shared" si="2"/>
         <v>0:05:31</v>
       </c>
+      <c r="AD32">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE32" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF32" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG32" s="3">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AH32" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -9437,8 +10121,28 @@
         <f t="shared" si="2"/>
         <v>0:01:25</v>
       </c>
+      <c r="AD33">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="AE33" s="3">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="AF33" s="3">
+        <f t="shared" si="5"/>
+        <v>1</v>
+      </c>
+      <c r="AG33" s="3">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="AH33" s="3">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -9514,19 +10218,39 @@
       </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="11">
-        <f t="shared" ref="AA34:AA65" si="3">SUM(F34,H34,K34, L34,N34,R34,(T34*7),(W34*7),Y34)/7</f>
+        <f t="shared" ref="AA34:AA65" si="8">SUM(F34,H34,K34, L34,N34,R34,(T34*7),(W34*7),Y34)/7</f>
         <v>14.928571428571429</v>
       </c>
       <c r="AB34" s="7">
-        <f t="shared" ref="AB34:AB65" si="4">AVERAGE(J34,P34,S34,V34,X34)</f>
+        <f t="shared" ref="AB34:AB65" si="9">AVERAGE(J34,P34,S34,V34,X34)</f>
         <v>5.4</v>
       </c>
       <c r="AC34" t="str">
-        <f t="shared" ref="AC34:AC65" si="5">TEXT(C34-B34, "h:mm:ss")</f>
+        <f t="shared" ref="AC34:AC65" si="10">TEXT(C34-B34, "h:mm:ss")</f>
         <v>0:01:54</v>
       </c>
+      <c r="AD34">
+        <f t="shared" ref="AD34:AD65" si="11">IF(F34&gt;=15, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE34" s="3">
+        <f t="shared" ref="AE34:AE65" si="12">IF(G34&gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF34" s="3">
+        <f t="shared" ref="AF34:AF65" si="13">IF(G34&gt;1, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AG34" s="3">
+        <f t="shared" ref="AG34:AG65" si="14">IF(F34&gt;40, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH34" s="3">
+        <f t="shared" ref="AH34:AH65" si="15">IF(I34&gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -9602,19 +10326,39 @@
       </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>17</v>
       </c>
       <c r="AB35" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>4.8</v>
       </c>
       <c r="AC35" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:52</v>
       </c>
+      <c r="AD35">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE35" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF35" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG35" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH35" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -9690,19 +10434,39 @@
       </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>11.714285714285714</v>
       </c>
       <c r="AB36" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AC36" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:27</v>
       </c>
+      <c r="AD36">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE36" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF36" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG36" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH36" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -9778,19 +10542,39 @@
       </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>20.714285714285715</v>
       </c>
       <c r="AB37" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC37" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:05</v>
       </c>
+      <c r="AD37">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE37" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF37" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG37" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH37" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -9866,19 +10650,39 @@
       </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>22.714285714285715</v>
       </c>
       <c r="AB38" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AC38" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:31</v>
       </c>
+      <c r="AD38">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE38" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF38" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG38" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH38" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -9954,19 +10758,39 @@
       </c>
       <c r="Z39" s="2"/>
       <c r="AA39" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>15.142857142857142</v>
       </c>
       <c r="AB39" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6.8</v>
       </c>
       <c r="AC39" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:34</v>
       </c>
+      <c r="AD39">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="AE39" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF39" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG39" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH39" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10042,19 +10866,39 @@
       </c>
       <c r="Z40" s="2"/>
       <c r="AA40" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14.428571428571429</v>
       </c>
       <c r="AB40" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AC40" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:35</v>
       </c>
+      <c r="AD40">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE40" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF40" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG40" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH40" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -10130,19 +10974,39 @@
       </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>18.571428571428573</v>
       </c>
       <c r="AB41" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC41" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:17</v>
       </c>
+      <c r="AD41">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE41" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF41" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG41" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH41" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -10218,19 +11082,39 @@
       </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14.857142857142858</v>
       </c>
       <c r="AB42" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.2</v>
       </c>
       <c r="AC42" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:57</v>
       </c>
+      <c r="AD42">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE42" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF42" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG42" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH42" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -10306,19 +11190,39 @@
       </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>17.714285714285715</v>
       </c>
       <c r="AB43" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6.4</v>
       </c>
       <c r="AC43" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:57</v>
       </c>
+      <c r="AD43">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE43" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF43" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG43" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH43" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -10394,19 +11298,39 @@
       </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>13.142857142857142</v>
       </c>
       <c r="AB44" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC44" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:04:04</v>
       </c>
+      <c r="AD44">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE44" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF44" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG44" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH44" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -10482,19 +11406,39 @@
       </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>17.214285714285715</v>
       </c>
       <c r="AB45" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AC45" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:46</v>
       </c>
+      <c r="AD45">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE45" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF45" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG45" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH45" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -10570,19 +11514,39 @@
       </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>18.857142857142858</v>
       </c>
       <c r="AB46" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>4.5999999999999996</v>
       </c>
       <c r="AC46" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:20</v>
       </c>
+      <c r="AD46">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE46" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF46" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG46" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH46" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -10658,19 +11622,39 @@
       </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>15.285714285714286</v>
       </c>
       <c r="AB47" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>7.6</v>
       </c>
       <c r="AC47" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:27</v>
       </c>
+      <c r="AD47">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE47" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF47" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG47" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH47" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -10746,19 +11730,39 @@
       </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>22.714285714285715</v>
       </c>
       <c r="AB48" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AC48" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:42</v>
       </c>
+      <c r="AD48">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE48" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF48" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG48" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH48" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -10834,19 +11838,39 @@
       </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>20.571428571428573</v>
       </c>
       <c r="AB49" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
       <c r="AC49" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:43</v>
       </c>
+      <c r="AD49">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE49" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF49" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG49" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH49" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -10922,19 +11946,39 @@
       </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14.285714285714286</v>
       </c>
       <c r="AB50" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AC50" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:04:35</v>
       </c>
+      <c r="AD50">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE50" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF50" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG50" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH50" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11010,19 +12054,39 @@
       </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>24.857142857142858</v>
       </c>
       <c r="AB51" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>3.4</v>
       </c>
       <c r="AC51" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:04:48</v>
       </c>
+      <c r="AD51">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE51" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF51" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG51" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH51" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11098,19 +12162,39 @@
       </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14.428571428571429</v>
       </c>
       <c r="AB52" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.6</v>
       </c>
       <c r="AC52" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:45</v>
       </c>
+      <c r="AD52">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE52" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF52" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG52" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH52" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="53" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11186,19 +12270,39 @@
       </c>
       <c r="Z53" s="2"/>
       <c r="AA53" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>14.857142857142858</v>
       </c>
       <c r="AB53" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.2</v>
       </c>
       <c r="AC53" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:57</v>
       </c>
+      <c r="AD53">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE53" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF53" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG53" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH53" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11274,19 +12378,39 @@
       </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>18.571428571428573</v>
       </c>
       <c r="AB54" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AC54" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:31</v>
       </c>
+      <c r="AD54">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE54" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF54" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG54" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH54" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="55" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11362,19 +12486,39 @@
       </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>16.857142857142858</v>
       </c>
       <c r="AB55" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC55" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:07</v>
       </c>
+      <c r="AD55">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE55" s="3">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="AF55" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG55" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH55" s="3">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11450,19 +12594,39 @@
       </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>19.571428571428573</v>
       </c>
       <c r="AB56" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AC56" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:03:05</v>
       </c>
+      <c r="AD56">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE56" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF56" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG56" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH56" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="57" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11538,19 +12702,39 @@
       </c>
       <c r="Z57" s="2"/>
       <c r="AA57" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>16</v>
       </c>
       <c r="AB57" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>4.2</v>
       </c>
       <c r="AC57" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:04:19</v>
       </c>
+      <c r="AD57">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE57" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF57" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG57" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH57" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="58" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11626,19 +12810,39 @@
       </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>12.285714285714286</v>
       </c>
       <c r="AB58" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.4</v>
       </c>
       <c r="AC58" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:41</v>
       </c>
+      <c r="AD58">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE58" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF58" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG58" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH58" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11714,19 +12918,39 @@
       </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>18.142857142857142</v>
       </c>
       <c r="AB59" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC59" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:09</v>
       </c>
+      <c r="AD59">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE59" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF59" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG59" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH59" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="60" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11802,19 +13026,39 @@
       </c>
       <c r="Z60" s="2"/>
       <c r="AA60" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>15.071428571428571</v>
       </c>
       <c r="AB60" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.2</v>
       </c>
       <c r="AC60" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1:15:04</v>
       </c>
+      <c r="AD60">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE60" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF60" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG60" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH60" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="61" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11890,19 +13134,39 @@
       </c>
       <c r="Z61" s="2"/>
       <c r="AA61" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>21.571428571428573</v>
       </c>
       <c r="AB61" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6.6</v>
       </c>
       <c r="AC61" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:35</v>
       </c>
+      <c r="AD61">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE61" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF61" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG61" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH61" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11978,19 +13242,39 @@
       </c>
       <c r="Z62" s="2"/>
       <c r="AA62" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>16.714285714285715</v>
       </c>
       <c r="AB62" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6</v>
       </c>
       <c r="AC62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:42</v>
       </c>
+      <c r="AD62">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE62" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF62" s="3">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AG62" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH62" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -12066,19 +13350,39 @@
       </c>
       <c r="Z63" s="2"/>
       <c r="AA63" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>19.857142857142858</v>
       </c>
       <c r="AB63" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>6.4</v>
       </c>
       <c r="AC63" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:48</v>
       </c>
+      <c r="AD63">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE63" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF63" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG63" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH63" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -12154,19 +13458,39 @@
       </c>
       <c r="Z64" s="2"/>
       <c r="AA64" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>13.571428571428571</v>
       </c>
       <c r="AB64" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>2</v>
       </c>
       <c r="AC64" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:01:57</v>
       </c>
+      <c r="AD64">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE64" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF64" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG64" s="3">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="AH64" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -12242,19 +13566,39 @@
       </c>
       <c r="Z65" s="2"/>
       <c r="AA65" s="11">
-        <f t="shared" si="3"/>
+        <f t="shared" si="8"/>
         <v>15.857142857142858</v>
       </c>
       <c r="AB65" s="7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="9"/>
         <v>5.8</v>
       </c>
       <c r="AC65" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>0:02:11</v>
       </c>
+      <c r="AD65">
+        <f t="shared" si="11"/>
+        <v>1</v>
+      </c>
+      <c r="AE65" s="3">
+        <f t="shared" si="12"/>
+        <v>1</v>
+      </c>
+      <c r="AF65" s="3">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="AG65" s="3">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="AH65" s="3">
+        <f t="shared" si="15"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -12330,19 +13674,39 @@
       </c>
       <c r="Z66" s="2"/>
       <c r="AA66" s="11">
-        <f t="shared" ref="AA66:AA91" si="6">SUM(F66,H66,K66, L66,N66,R66,(T66*7),(W66*7),Y66)/7</f>
+        <f t="shared" ref="AA66:AA91" si="16">SUM(F66,H66,K66, L66,N66,R66,(T66*7),(W66*7),Y66)/7</f>
         <v>16.285714285714285</v>
       </c>
       <c r="AB66" s="7">
-        <f t="shared" ref="AB66:AB91" si="7">AVERAGE(J66,P66,S66,V66,X66)</f>
+        <f t="shared" ref="AB66:AB91" si="17">AVERAGE(J66,P66,S66,V66,X66)</f>
         <v>6.4</v>
       </c>
       <c r="AC66" t="str">
-        <f t="shared" ref="AC66:AC91" si="8">TEXT(C66-B66, "h:mm:ss")</f>
+        <f t="shared" ref="AC66:AC91" si="18">TEXT(C66-B66, "h:mm:ss")</f>
         <v>0:02:04</v>
       </c>
+      <c r="AD66">
+        <f t="shared" ref="AD66:AD91" si="19">IF(F66&gt;=15, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AE66" s="3">
+        <f t="shared" ref="AE66:AE91" si="20">IF(G66&gt;0, 1, 0)</f>
+        <v>1</v>
+      </c>
+      <c r="AF66" s="3">
+        <f t="shared" ref="AF66:AF91" si="21">IF(G66&gt;1, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AG66" s="3">
+        <f t="shared" ref="AG66:AG91" si="22">IF(F66&gt;40, 1, 0)</f>
+        <v>0</v>
+      </c>
+      <c r="AH66" s="3">
+        <f t="shared" ref="AH66:AH91" si="23">IF(I66&gt;0, 1, 0)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -12418,19 +13782,39 @@
       </c>
       <c r="Z67" s="2"/>
       <c r="AA67" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>18.571428571428573</v>
       </c>
       <c r="AB67" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="AC67" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:05:57</v>
       </c>
+      <c r="AD67">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE67" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF67" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG67" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH67" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -12506,19 +13890,39 @@
       </c>
       <c r="Z68" s="2"/>
       <c r="AA68" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>13.285714285714286</v>
       </c>
       <c r="AB68" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.8</v>
       </c>
       <c r="AC68" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:47</v>
       </c>
+      <c r="AD68">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE68" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF68" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG68" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH68" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -12594,19 +13998,39 @@
       </c>
       <c r="Z69" s="2"/>
       <c r="AA69" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>20.428571428571427</v>
       </c>
       <c r="AB69" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="AC69" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:30</v>
       </c>
+      <c r="AD69">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE69" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF69" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG69" s="3">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AH69" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="70" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -12682,19 +14106,39 @@
       </c>
       <c r="Z70" s="2"/>
       <c r="AA70" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>12</v>
       </c>
       <c r="AB70" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4.2</v>
       </c>
       <c r="AC70" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:07:13</v>
       </c>
+      <c r="AD70">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE70" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF70" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG70" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH70" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -12770,19 +14214,39 @@
       </c>
       <c r="Z71" s="2"/>
       <c r="AA71" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>13.428571428571429</v>
       </c>
       <c r="AB71" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="AC71" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:07:55</v>
       </c>
+      <c r="AD71">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE71" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF71" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG71" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH71" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>71</v>
       </c>
@@ -12858,19 +14322,39 @@
       </c>
       <c r="Z72" s="2"/>
       <c r="AA72" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>19.214285714285715</v>
       </c>
       <c r="AB72" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.2</v>
       </c>
       <c r="AC72" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:07:13</v>
       </c>
+      <c r="AD72">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE72" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF72" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG72" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH72" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>72</v>
       </c>
@@ -12946,19 +14430,39 @@
       </c>
       <c r="Z73" s="2"/>
       <c r="AA73" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>44.714285714285715</v>
       </c>
       <c r="AB73" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>8.1999999999999993</v>
       </c>
       <c r="AC73" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:00</v>
       </c>
+      <c r="AD73">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE73" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF73" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG73" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH73" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>73</v>
       </c>
@@ -13034,19 +14538,39 @@
       </c>
       <c r="Z74" s="2"/>
       <c r="AA74" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>17.571428571428573</v>
       </c>
       <c r="AB74" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.2</v>
       </c>
       <c r="AC74" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:31</v>
       </c>
+      <c r="AD74">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE74" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF74" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG74" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH74" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>74</v>
       </c>
@@ -13122,19 +14646,39 @@
       </c>
       <c r="Z75" s="2"/>
       <c r="AA75" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>17.714285714285715</v>
       </c>
       <c r="AB75" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>3</v>
       </c>
       <c r="AC75" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:01:55</v>
       </c>
+      <c r="AD75">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE75" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF75" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG75" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH75" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>75</v>
       </c>
@@ -13210,19 +14754,39 @@
       </c>
       <c r="Z76" s="2"/>
       <c r="AA76" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>15.428571428571429</v>
       </c>
       <c r="AB76" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>6</v>
       </c>
       <c r="AC76" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:51</v>
       </c>
+      <c r="AD76">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE76" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF76" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG76" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH76" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>76</v>
       </c>
@@ -13298,19 +14862,39 @@
       </c>
       <c r="Z77" s="2"/>
       <c r="AA77" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>10.714285714285714</v>
       </c>
       <c r="AB77" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>6.6</v>
       </c>
       <c r="AC77" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:54</v>
       </c>
+      <c r="AD77">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE77" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF77" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG77" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH77" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>77</v>
       </c>
@@ -13386,19 +14970,39 @@
       </c>
       <c r="Z78" s="2"/>
       <c r="AA78" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>14.857142857142858</v>
       </c>
       <c r="AB78" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.6</v>
       </c>
       <c r="AC78" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:41</v>
       </c>
+      <c r="AD78">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE78" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF78" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG78" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH78" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>78</v>
       </c>
@@ -13474,19 +15078,39 @@
       </c>
       <c r="Z79" s="2"/>
       <c r="AA79" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>12.285714285714286</v>
       </c>
       <c r="AB79" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.6</v>
       </c>
       <c r="AC79" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:16</v>
       </c>
+      <c r="AD79">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE79" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF79" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG79" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH79" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>79</v>
       </c>
@@ -13562,19 +15186,39 @@
       </c>
       <c r="Z80" s="2"/>
       <c r="AA80" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>14.285714285714286</v>
       </c>
       <c r="AB80" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>3.6</v>
       </c>
       <c r="AC80" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:03</v>
       </c>
+      <c r="AD80">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE80" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF80" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG80" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH80" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>80</v>
       </c>
@@ -13650,19 +15294,39 @@
       </c>
       <c r="Z81" s="2"/>
       <c r="AA81" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>18.571428571428573</v>
       </c>
       <c r="AB81" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4.2</v>
       </c>
       <c r="AC81" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:00</v>
       </c>
+      <c r="AD81">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE81" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AF81" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG81" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH81" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>81</v>
       </c>
@@ -13738,19 +15402,39 @@
       </c>
       <c r="Z82" s="2"/>
       <c r="AA82" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>18.214285714285715</v>
       </c>
       <c r="AB82" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.8</v>
       </c>
       <c r="AC82" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:52</v>
       </c>
+      <c r="AD82">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE82" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF82" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG82" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH82" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>82</v>
       </c>
@@ -13826,19 +15510,39 @@
       </c>
       <c r="Z83" s="2"/>
       <c r="AA83" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>23.285714285714285</v>
       </c>
       <c r="AB83" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>6.4</v>
       </c>
       <c r="AC83" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:16</v>
       </c>
+      <c r="AD83">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE83" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AF83" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG83" s="3">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AH83" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>83</v>
       </c>
@@ -13914,19 +15618,39 @@
       </c>
       <c r="Z84" s="2"/>
       <c r="AA84" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>28.071428571428573</v>
       </c>
       <c r="AB84" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>7.2</v>
       </c>
       <c r="AC84" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:21:41</v>
       </c>
+      <c r="AD84">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE84" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF84" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG84" s="3">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AH84" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>84</v>
       </c>
@@ -14002,19 +15726,39 @@
       </c>
       <c r="Z85" s="2"/>
       <c r="AA85" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>24.428571428571427</v>
       </c>
       <c r="AB85" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>6.4</v>
       </c>
       <c r="AC85" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:01:43</v>
       </c>
+      <c r="AD85">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE85" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF85" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG85" s="3">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AH85" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>85</v>
       </c>
@@ -14090,19 +15834,39 @@
       </c>
       <c r="Z86" s="2"/>
       <c r="AA86" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>15.857142857142858</v>
       </c>
       <c r="AB86" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="AC86" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:03:31</v>
       </c>
+      <c r="AD86">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE86" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF86" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG86" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH86" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -14178,19 +15942,39 @@
       </c>
       <c r="Z87" s="2"/>
       <c r="AA87" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>22.857142857142858</v>
       </c>
       <c r="AB87" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="AC87" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:04:56</v>
       </c>
+      <c r="AD87">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE87" s="3">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="AF87" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG87" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH87" s="3">
+        <f t="shared" si="23"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>87</v>
       </c>
@@ -14266,19 +16050,39 @@
       </c>
       <c r="Z88" s="2"/>
       <c r="AA88" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>16.285714285714285</v>
       </c>
       <c r="AB88" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4.8</v>
       </c>
       <c r="AC88" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:01:43</v>
       </c>
+      <c r="AD88">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE88" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF88" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG88" s="3">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="AH88" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>88</v>
       </c>
@@ -14354,19 +16158,39 @@
       </c>
       <c r="Z89" s="2"/>
       <c r="AA89" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>17.857142857142858</v>
       </c>
       <c r="AB89" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5.2</v>
       </c>
       <c r="AC89" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:02:15</v>
       </c>
+      <c r="AD89">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE89" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF89" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG89" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH89" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>89</v>
       </c>
@@ -14442,19 +16266,39 @@
       </c>
       <c r="Z90" s="2"/>
       <c r="AA90" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>17.428571428571427</v>
       </c>
       <c r="AB90" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>5</v>
       </c>
       <c r="AC90" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:12:21</v>
       </c>
+      <c r="AD90">
+        <f t="shared" si="19"/>
+        <v>1</v>
+      </c>
+      <c r="AE90" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF90" s="3">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="AG90" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH90" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>90</v>
       </c>
@@ -14530,16 +16374,36 @@
       </c>
       <c r="Z91" s="2"/>
       <c r="AA91" s="11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="16"/>
         <v>14.428571428571429</v>
       </c>
       <c r="AB91" s="7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="17"/>
         <v>4</v>
       </c>
       <c r="AC91" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="18"/>
         <v>0:06:14</v>
+      </c>
+      <c r="AD91">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="AE91" s="3">
+        <f t="shared" si="20"/>
+        <v>1</v>
+      </c>
+      <c r="AF91" s="3">
+        <f t="shared" si="21"/>
+        <v>1</v>
+      </c>
+      <c r="AG91" s="3">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="AH91" s="3">
+        <f t="shared" si="23"/>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>